<commit_message>
Added and modified fields
</commit_message>
<xml_diff>
--- a/PhishingData.xlsx
+++ b/PhishingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eddie\Desktop\Cyber Security\Webform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86AC431-A3F4-4EDD-814C-54D973897C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49673749-D849-48C8-8221-07A9D51795A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="2640" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20268" yWindow="1836" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>fname</t>
   </si>
   <si>
-    <t>myemail</t>
-  </si>
-  <si>
     <t>myphone</t>
   </si>
   <si>
@@ -41,6 +38,15 @@
   </si>
   <si>
     <t>lname</t>
+  </si>
+  <si>
+    <t>Recipient</t>
+  </si>
+  <si>
+    <t>myusername</t>
+  </si>
+  <si>
+    <t>Email Sent</t>
   </si>
 </sst>
 </file>
@@ -302,7 +308,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -310,29 +316,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>